<commit_message>
Addition of case study examples.
</commit_message>
<xml_diff>
--- a/01_Input/Sample_Input/Case_Study/TCRBiasExamples.xlsx
+++ b/01_Input/Sample_Input/Case_Study/TCRBiasExamples.xlsx
@@ -1,21 +1,22 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10215"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10313"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/austinseamann/Library/Mobile Documents/com~apple~CloudDocs/School/BioI-Lab/TRain/01_Input/Sample_Input/Case_Study/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7EDE951A-CD6F-8342-9AB2-2D910140DE5C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B4B18ACE-519E-5940-ADC5-39667B8DD4E9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="500" windowWidth="16800" windowHeight="20500" xr2:uid="{E355CE78-08F7-2A4D-A172-AD1B8A80E5BC}"/>
-    <workbookView xWindow="16800" yWindow="500" windowWidth="16800" windowHeight="20500" activeTab="1" xr2:uid="{F796C56A-A9F5-5245-84AF-A3AD1A877762}"/>
+    <workbookView xWindow="16800" yWindow="500" windowWidth="16800" windowHeight="20500" activeTab="2" xr2:uid="{F796C56A-A9F5-5245-84AF-A3AD1A877762}"/>
   </bookViews>
   <sheets>
     <sheet name="TCRs" sheetId="1" r:id="rId1"/>
     <sheet name="SeqInfo" sheetId="2" r:id="rId2"/>
+    <sheet name="Runs" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="181029"/>
   <extLst>
@@ -37,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="163" uniqueCount="124">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="236" uniqueCount="140">
   <si>
     <t>Pathogen</t>
   </si>
@@ -409,6 +410,54 @@
   </si>
   <si>
     <t>TRAJ21*01</t>
+  </si>
+  <si>
+    <t>AS01_1</t>
+  </si>
+  <si>
+    <t>AS01_2</t>
+  </si>
+  <si>
+    <t>AS01</t>
+  </si>
+  <si>
+    <t>GLCTLVAML</t>
+  </si>
+  <si>
+    <t>20-1</t>
+  </si>
+  <si>
+    <t>5</t>
+  </si>
+  <si>
+    <t>31</t>
+  </si>
+  <si>
+    <t>BMLF1_280_288</t>
+  </si>
+  <si>
+    <t>Equal Bias: https://journals.plos.org/plospathogens/article?id=10.1371/journal.ppat.1001198</t>
+  </si>
+  <si>
+    <t>CAEDFNARLMF</t>
+  </si>
+  <si>
+    <t>TRAJ31*01</t>
+  </si>
+  <si>
+    <t>TRBV20-1*01</t>
+  </si>
+  <si>
+    <t>CSARTGVGNTIYF</t>
+  </si>
+  <si>
+    <t>TRBJ1-3*01</t>
+  </si>
+  <si>
+    <t>CAEDKDARLMF</t>
+  </si>
+  <si>
+    <t>CSARDRIGNTIYF</t>
   </si>
 </sst>
 </file>
@@ -431,12 +480,18 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -451,10 +506,11 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="49" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -769,10 +825,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{464BEE6F-3D7A-B847-88AB-D2E7FA5F267C}">
-  <dimension ref="A1:J8"/>
+  <dimension ref="A1:J9"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A8" sqref="A8"/>
+      <selection activeCell="D9" sqref="D9"/>
     </sheetView>
     <sheetView workbookViewId="1">
       <selection activeCell="H9" sqref="H9"/>
@@ -822,7 +878,7 @@
       </c>
     </row>
     <row r="2" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A2" s="1" t="s">
+      <c r="A2" s="3" t="s">
         <v>9</v>
       </c>
       <c r="B2" s="1" t="s">
@@ -960,7 +1016,7 @@
       </c>
     </row>
     <row r="8" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A8" s="1" t="s">
+      <c r="A8" s="3" t="s">
         <v>49</v>
       </c>
       <c r="B8" s="1" t="s">
@@ -986,6 +1042,38 @@
       </c>
       <c r="J8" s="1" t="s">
         <v>50</v>
+      </c>
+    </row>
+    <row r="9" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A9" s="3" t="s">
+        <v>126</v>
+      </c>
+      <c r="B9" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="C9" s="1" t="s">
+        <v>131</v>
+      </c>
+      <c r="D9" s="1" t="s">
+        <v>127</v>
+      </c>
+      <c r="E9" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="F9" s="1" t="s">
+        <v>129</v>
+      </c>
+      <c r="G9" s="1" t="s">
+        <v>130</v>
+      </c>
+      <c r="H9" s="1" t="s">
+        <v>128</v>
+      </c>
+      <c r="I9" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="J9" s="1" t="s">
+        <v>132</v>
       </c>
     </row>
   </sheetData>
@@ -995,13 +1083,13 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C01FB5A0-DA7A-9F45-B559-B64DB1A37191}">
-  <dimension ref="A1:H15"/>
+  <dimension ref="A1:H17"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="F10" sqref="F10"/>
     </sheetView>
-    <sheetView tabSelected="1" workbookViewId="1">
-      <selection activeCell="G13" sqref="G13"/>
+    <sheetView workbookViewId="1">
+      <selection activeCell="A16" sqref="A16:H17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1397,6 +1485,253 @@
         <v>68</v>
       </c>
     </row>
+    <row r="16" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A16" t="s">
+        <v>124</v>
+      </c>
+      <c r="B16" t="s">
+        <v>112</v>
+      </c>
+      <c r="C16" t="s">
+        <v>133</v>
+      </c>
+      <c r="D16" t="s">
+        <v>134</v>
+      </c>
+      <c r="E16" t="s">
+        <v>135</v>
+      </c>
+      <c r="F16" t="s">
+        <v>136</v>
+      </c>
+      <c r="G16" t="s">
+        <v>137</v>
+      </c>
+      <c r="H16">
+        <v>1543</v>
+      </c>
+    </row>
+    <row r="17" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A17" t="s">
+        <v>125</v>
+      </c>
+      <c r="B17" t="s">
+        <v>112</v>
+      </c>
+      <c r="C17" t="s">
+        <v>138</v>
+      </c>
+      <c r="D17" t="s">
+        <v>134</v>
+      </c>
+      <c r="E17" t="s">
+        <v>135</v>
+      </c>
+      <c r="F17" t="s">
+        <v>139</v>
+      </c>
+      <c r="G17" t="s">
+        <v>137</v>
+      </c>
+      <c r="H17">
+        <v>1546</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A1F8D762-DA80-F04F-9940-53BF35454256}">
+  <dimension ref="A1:H7"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="1">
+      <selection activeCell="F10" sqref="F10"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetData>
+    <row r="1" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A1" t="s">
+        <v>51</v>
+      </c>
+      <c r="B1" t="s">
+        <v>5</v>
+      </c>
+      <c r="C1" t="s">
+        <v>52</v>
+      </c>
+      <c r="D1" t="s">
+        <v>6</v>
+      </c>
+      <c r="E1" t="s">
+        <v>7</v>
+      </c>
+      <c r="F1" t="s">
+        <v>53</v>
+      </c>
+      <c r="G1" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A2" t="s">
+        <v>54</v>
+      </c>
+      <c r="B2" t="s">
+        <v>58</v>
+      </c>
+      <c r="C2" t="s">
+        <v>59</v>
+      </c>
+      <c r="D2" t="s">
+        <v>60</v>
+      </c>
+      <c r="E2" t="s">
+        <v>55</v>
+      </c>
+      <c r="F2" t="s">
+        <v>56</v>
+      </c>
+      <c r="G2" t="s">
+        <v>57</v>
+      </c>
+      <c r="H2">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A3" t="s">
+        <v>61</v>
+      </c>
+      <c r="B3" t="s">
+        <v>58</v>
+      </c>
+      <c r="C3" t="s">
+        <v>72</v>
+      </c>
+      <c r="D3" t="s">
+        <v>73</v>
+      </c>
+      <c r="E3" t="s">
+        <v>55</v>
+      </c>
+      <c r="F3" t="s">
+        <v>71</v>
+      </c>
+      <c r="G3" t="s">
+        <v>57</v>
+      </c>
+      <c r="H3">
+        <v>259</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A4" t="s">
+        <v>114</v>
+      </c>
+      <c r="B4" t="s">
+        <v>116</v>
+      </c>
+      <c r="C4" t="s">
+        <v>117</v>
+      </c>
+      <c r="D4" t="s">
+        <v>65</v>
+      </c>
+      <c r="E4" t="s">
+        <v>55</v>
+      </c>
+      <c r="F4" t="s">
+        <v>118</v>
+      </c>
+      <c r="G4" t="s">
+        <v>83</v>
+      </c>
+      <c r="H4">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A5" t="s">
+        <v>115</v>
+      </c>
+      <c r="B5" t="s">
+        <v>116</v>
+      </c>
+      <c r="C5" t="s">
+        <v>117</v>
+      </c>
+      <c r="D5" t="s">
+        <v>65</v>
+      </c>
+      <c r="E5" t="s">
+        <v>55</v>
+      </c>
+      <c r="F5" t="s">
+        <v>119</v>
+      </c>
+      <c r="G5" t="s">
+        <v>120</v>
+      </c>
+      <c r="H5">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A6" t="s">
+        <v>124</v>
+      </c>
+      <c r="B6" t="s">
+        <v>112</v>
+      </c>
+      <c r="C6" t="s">
+        <v>133</v>
+      </c>
+      <c r="D6" t="s">
+        <v>134</v>
+      </c>
+      <c r="E6" t="s">
+        <v>135</v>
+      </c>
+      <c r="F6" t="s">
+        <v>136</v>
+      </c>
+      <c r="G6" t="s">
+        <v>137</v>
+      </c>
+      <c r="H6">
+        <v>1543</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A7" t="s">
+        <v>125</v>
+      </c>
+      <c r="B7" t="s">
+        <v>112</v>
+      </c>
+      <c r="C7" t="s">
+        <v>138</v>
+      </c>
+      <c r="D7" t="s">
+        <v>134</v>
+      </c>
+      <c r="E7" t="s">
+        <v>135</v>
+      </c>
+      <c r="F7" t="s">
+        <v>139</v>
+      </c>
+      <c r="G7" t="s">
+        <v>137</v>
+      </c>
+      <c r="H7">
+        <v>1546</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>